<commit_message>
adaptacion css de la pagina
</commit_message>
<xml_diff>
--- a/Documentacion/Tareas a realizar.xlsx
+++ b/Documentacion/Tareas a realizar.xlsx
@@ -78,12 +78,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="I5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AGAPITO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Se ha completado y se ha abanzado la parte de mañana.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>semana 1</t>
   </si>
@@ -519,12 +543,72 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -543,9 +627,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -580,63 +661,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -921,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,15 +959,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
       <c r="J2" s="14" t="s">
         <v>28</v>
       </c>
@@ -955,10 +979,10 @@
       <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="46"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="12" t="s">
         <v>9</v>
       </c>
@@ -969,7 +993,7 @@
       <c r="I3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="38" t="s">
         <v>29</v>
       </c>
     </row>
@@ -977,67 +1001,69 @@
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="56" t="s">
+      <c r="I4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="17"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="17"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="51" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="53"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="15"/>
-      <c r="J6" s="17"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="55" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="15"/>
-      <c r="J7" s="17"/>
+      <c r="J7" s="38"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
@@ -1058,82 +1084,85 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="J10">
+        <v>7277</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
@@ -1154,177 +1183,159 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="28" t="s">
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="29"/>
+      <c r="H21" s="48"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19" t="s">
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="41"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="11"/>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="24"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="44"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="24"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="24"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="44"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="19" t="s">
+      <c r="C30" s="45"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="21"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="41"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19" t="s">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="21"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C19:H19"/>
     <mergeCell ref="J3:J7"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="E31:H31"/>
@@ -1341,6 +1352,24 @@
     <mergeCell ref="E23:H23"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>